<commit_message>
Removed excel tmp file, formatted spawn data
</commit_message>
<xml_diff>
--- a/2048 spawn data.xlsx
+++ b/2048 spawn data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\2048\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\2048-fork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DE5C605-5367-42E9-8AE0-96E5967DA805}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C270ABC-A095-44E4-8278-89740DBA412B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{9E1EE7F9-71E3-4A88-B341-D49C2BB1AAC2}"/>
   </bookViews>
@@ -30,17 +30,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Playing</t>
+  </si>
+  <si>
+    <t>Counts</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>All tiles</t>
+  </si>
+  <si>
+    <t>Repeatedly hitting new game</t>
+  </si>
+  <si>
+    <t>Fraction 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,99 +408,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D4C172-C99D-4758-BB6B-032F78DECD29}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>2</v>
-      </c>
-      <c r="B1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <f>SUM(A3:A300)</f>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f>SUM(A6:A300)</f>
         <v>102</v>
       </c>
-      <c r="B2">
-        <f>SUM(B3:B300)</f>
+      <c r="B5">
+        <f>SUM(B6:B300)</f>
         <v>8</v>
       </c>
-      <c r="C2">
-        <f>SUM(A2:B2)</f>
+      <c r="C5">
+        <f>SUM(A5:B5)</f>
         <v>110</v>
       </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="D5">
+        <f>B5/C5</f>
+        <v>7.2727272727272724E-2</v>
+      </c>
+      <c r="F5">
+        <f>SUM(F6:F400)</f>
+        <v>89</v>
+      </c>
+      <c r="G5">
+        <f>SUM(G6:G400)</f>
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <f>F5+G5</f>
+        <v>95</v>
+      </c>
+      <c r="I5">
+        <f>G5/H5</f>
+        <v>6.3157894736842107E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>92</v>
       </c>
-      <c r="B3">
+      <c r="B6">
         <v>8</v>
       </c>
-      <c r="F3">
-        <f>SUM(F4:F400)</f>
-        <v>89</v>
-      </c>
-      <c r="G3">
-        <f>SUM(G4:G400)</f>
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <f>6/89</f>
-        <v>6.741573033707865E-2</v>
-      </c>
-      <c r="J3">
-        <f>8/110</f>
-        <v>7.2727272727272724E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <f>1/15</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
       <c r="F6">
         <v>1</v>
       </c>
@@ -484,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -495,7 +523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -506,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -517,23 +545,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -541,7 +575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -549,17 +583,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
       <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1</v>
+      </c>
       <c r="F15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1</v>
+      </c>
       <c r="F16">
         <v>1</v>
       </c>
@@ -941,6 +984,16 @@
     </row>
     <row r="92" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F94">
         <v>1</v>
       </c>
     </row>

</xml_diff>